<commit_message>
Rename FontCache to something more sensible. Use interface, so I can have two implementations at once and compare results them when needed.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
@@ -728,10 +728,10 @@
   <x:cols>
     <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="7.980625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="9.000625" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="8.580625" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="11.950625" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="15.590625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="8.930625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="8.520625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="11.840625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="15.550625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="2" spans="1:6">

</xml_diff>

<commit_message>
Adressing font width and height issues
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
@@ -727,11 +727,11 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="6.640625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="6.570625" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="7.240625" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="10.100625" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="12.270625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="7.300625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="7.240625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="7.840625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="10.340625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="12.310625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="2" spans="1:6">

</xml_diff>

<commit_message>
Fixed more column size adjusting issues
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
@@ -727,11 +727,11 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="7.300625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="7.240625" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="7.840625" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="10.340625" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="12.310625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="9.250625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="10.290625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="9.950625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="13.220625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="16.820625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="2" spans="1:6">

</xml_diff>

<commit_message>
Moving from "Verdana" to "DejaVu Serif"
Skiasharp found no "Verdana" on ubuntu and falls back to some default.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
@@ -727,11 +727,11 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="9.250625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="10.290625" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="9.950625" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="13.220625" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="16.820625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="9.620625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="10.710625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="10.360625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="13.780625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="17.560625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="2" spans="1:6">

</xml_diff>

<commit_message>
Switch to the engine that uses Calibri font for font measurement. The embedded font is a kept and should be used on non-Windows environments that don't want to use more specialized engine.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
@@ -727,9 +727,9 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="7.980625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="7.870625" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="9.000625" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="8.580625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="8.440625" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="11.950625" style="0" customWidth="1"/>
     <x:col min="6" max="6" width="15.590625" style="0" customWidth="1"/>
   </x:cols>

</xml_diff>

<commit_message>
Update test files to merged graphic engine that uses SixLabors.Fonts library.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
@@ -727,11 +727,11 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="7.870625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="9.000625" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="8.440625" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="11.950625" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="15.590625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="7.990625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="9.040625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="8.520625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="11.920625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="15.720625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="2" spans="1:6">

</xml_diff>